<commit_message>
Made a few runs with BS32. Last run: 5 mins
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -143,8 +143,8 @@
   </sheetPr>
   <dimension ref="B2:G52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -175,36 +175,48 @@
       <c r="C4" s="1" t="n">
         <v>0.1</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="E4" s="0" t="n">
         <f aca="false">4*D4</f>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="n">
         <v>0.01</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="E5" s="0" t="n">
         <f aca="false">4*D5</f>
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>86</v>
+      </c>
       <c r="E6" s="0" t="n">
         <f aca="false">4*D6</f>
-        <v>0</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1" t="n">
         <v>0.0001</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>195</v>
+      </c>
       <c r="E7" s="0" t="n">
         <f aca="false">4*D7</f>
-        <v>0</v>
+        <v>780</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,8 +470,8 @@
         <v>392</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">(141+141+143+153)/4</f>
-        <v>144.5</v>
+        <f aca="false">(191+2*193+203)/4</f>
+        <v>195</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,9 +659,12 @@
       <c r="C52" s="1" t="n">
         <v>1E-010</v>
       </c>
+      <c r="D52" s="0" t="n">
+        <v>193</v>
+      </c>
       <c r="E52" s="0" t="n">
         <f aca="false">13*D52</f>
-        <v>0</v>
+        <v>2509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made more runs with various integrators. Last BS32 run: 10 mins
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -144,7 +144,7 @@
   <dimension ref="B2:G52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -223,9 +223,12 @@
       <c r="C8" s="1" t="n">
         <v>1E-005</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>426</v>
+      </c>
       <c r="E8" s="0" t="n">
         <f aca="false">4*D8</f>
-        <v>0</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,8 +473,8 @@
         <v>392</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">(191+2*193+203)/4</f>
-        <v>195</v>
+        <f aca="false">(418+420+424+442)/4</f>
+        <v>426</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,36 +614,48 @@
       <c r="C47" s="1" t="n">
         <v>1E-005</v>
       </c>
+      <c r="D47" s="0" t="n">
+        <v>44</v>
+      </c>
       <c r="E47" s="0" t="n">
         <f aca="false">13*D47</f>
-        <v>0</v>
+        <v>572</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="n">
         <v>1E-006</v>
       </c>
+      <c r="D48" s="0" t="n">
+        <v>60</v>
+      </c>
       <c r="E48" s="0" t="n">
         <f aca="false">13*D48</f>
-        <v>0</v>
+        <v>780</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="n">
         <v>1E-007</v>
       </c>
+      <c r="D49" s="0" t="n">
+        <v>81</v>
+      </c>
       <c r="E49" s="0" t="n">
         <f aca="false">13*D49</f>
-        <v>0</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="n">
         <v>1E-008</v>
       </c>
+      <c r="D50" s="0" t="n">
+        <v>108</v>
+      </c>
       <c r="E50" s="0" t="n">
         <f aca="false">13*D50</f>
-        <v>0</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Made another BS32 run. Run took 20 min
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -56,6 +56,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,15 +145,15 @@
   <dimension ref="B2:G52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,9 +236,12 @@
       <c r="C9" s="1" t="n">
         <v>1E-006</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>924</v>
+      </c>
       <c r="E9" s="0" t="n">
         <f aca="false">4*D9</f>
-        <v>0</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,8 +477,8 @@
         <v>392</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">(418+420+424+442)/4</f>
-        <v>426</v>
+        <f aca="false">(909+911+917+957)/4</f>
+        <v>923.5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
One more BS32 run to go
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -145,15 +145,15 @@
   <dimension ref="B2:G52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,18 +248,24 @@
       <c r="C10" s="1" t="n">
         <v>1E-007</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>1991</v>
+      </c>
       <c r="E10" s="0" t="n">
         <f aca="false">4*D10</f>
-        <v>0</v>
+        <v>7964</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="n">
         <v>1E-008</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>4293</v>
+      </c>
       <c r="E11" s="0" t="n">
         <f aca="false">4*D11</f>
-        <v>0</v>
+        <v>17172</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,9 +281,12 @@
       <c r="C13" s="1" t="n">
         <v>1E-010</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>19929</v>
+      </c>
       <c r="E13" s="0" t="n">
         <f aca="false">4*D13</f>
-        <v>0</v>
+        <v>79716</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,9 +417,12 @@
       <c r="C26" s="1" t="n">
         <v>1E-010</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>613</v>
+      </c>
       <c r="E26" s="0" t="n">
         <f aca="false">8*D26</f>
-        <v>0</v>
+        <v>4904</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,8 +489,8 @@
         <v>392</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">(909+911+917+957)/4</f>
-        <v>923.5</v>
+        <f aca="false">(4223+4269+4457+4221)/4</f>
+        <v>4292.5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,9 +557,12 @@
       <c r="C39" s="1" t="n">
         <v>1E-010</v>
       </c>
+      <c r="D39" s="0" t="n">
+        <v>799</v>
+      </c>
       <c r="E39" s="0" t="n">
         <f aca="false">7*D39</f>
-        <v>0</v>
+        <v>5593</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Finished last run w BS32
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -56,7 +56,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,10 +141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G52"/>
+  <dimension ref="B2:G53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -272,9 +271,12 @@
       <c r="C12" s="1" t="n">
         <v>1E-009</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>9249</v>
+      </c>
       <c r="E12" s="0" t="n">
         <f aca="false">4*D12</f>
-        <v>0</v>
+        <v>36996</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,8 +491,8 @@
         <v>392</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">(4223+4269+4457+4221)/4</f>
-        <v>4292.5</v>
+        <f aca="false">(9099+9603+9199+9095)/4</f>
+        <v>9249</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,6 +701,12 @@
       <c r="E52" s="0" t="n">
         <f aca="false">13*D52</f>
         <v>2509</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="0" t="n">
+        <f aca="false">1.333*E52</f>
+        <v>3344.497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results section done. Next up: Discussion
</commit_message>
<xml_diff>
--- a/notebooks/doublegyre/integratorcalls.xlsx
+++ b/notebooks/doublegyre/integratorcalls.xlsx
@@ -141,10 +141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G53"/>
+  <dimension ref="B2:I54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -642,6 +642,10 @@
         <f aca="false">13*D47</f>
         <v>572</v>
       </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">911.915-15.83/2</f>
+        <v>904</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="n">
@@ -654,6 +658,10 @@
         <f aca="false">13*D48</f>
         <v>780</v>
       </c>
+      <c r="I48" s="0" t="n">
+        <f aca="false">407.915+292.33</f>
+        <v>700.245</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="n">
@@ -666,6 +674,10 @@
         <f aca="false">13*D49</f>
         <v>1053</v>
       </c>
+      <c r="I49" s="0" t="n">
+        <f aca="false">I48-15.383/2</f>
+        <v>692.5535</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="n">
@@ -678,6 +690,10 @@
         <f aca="false">13*D50</f>
         <v>1404</v>
       </c>
+      <c r="I50" s="0" t="n">
+        <f aca="false">38.755+15.383/2</f>
+        <v>46.4465</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="n">
@@ -703,10 +719,16 @@
         <v>2509</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="0" t="n">
-        <f aca="false">1.333*E52</f>
-        <v>3344.497</v>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="1" t="n">
+        <v>1E-012</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">13*D54</f>
+        <v>4485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>